<commit_message>
Auto-committed on 2022/02/11 週五
</commit_message>
<xml_diff>
--- a/Program/Other/URS會議審查紀錄/DbLayouts/XX-系統/TxDataLog.xlsx
+++ b/Program/Other/URS會議審查紀錄/DbLayouts/XX-系統/TxDataLog.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9132"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9012"/>
   </bookViews>
   <sheets>
     <sheet name="DBD" sheetId="1" r:id="rId1"/>
@@ -1050,7 +1050,7 @@
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.44140625" defaultRowHeight="15.6"/>
@@ -1265,7 +1265,7 @@
         <v>12</v>
       </c>
       <c r="E13" s="39">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="F13" s="40"/>
       <c r="G13" s="41"/>

</xml_diff>